<commit_message>
backup 13 Nov. 12:12
</commit_message>
<xml_diff>
--- a/experiment/param/experiment.xlsx
+++ b/experiment/param/experiment.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15648" activeTab="3"/>
+    <workbookView windowHeight="15648" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Graft Significance" sheetId="3" r:id="rId3"/>
     <sheet name="Robustness" sheetId="4" r:id="rId4"/>
+    <sheet name="Approximation" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>n_cluster</t>
   </si>
@@ -83,6 +84,30 @@
   </si>
   <si>
     <t>sorted</t>
+  </si>
+  <si>
+    <t>Approximation</t>
+  </si>
+  <si>
+    <t>Purity</t>
+  </si>
+  <si>
+    <t>Clustering Time</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>single_nn_search</t>
+  </si>
+  <si>
+    <t>single_elimination</t>
+  </si>
+  <si>
+    <t>capping</t>
+  </si>
+  <si>
+    <t>navigable_small_world_graphs</t>
   </si>
 </sst>
 </file>
@@ -93,8 +118,8 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.0000_ "/>
-    <numFmt numFmtId="177" formatCode="0.0_ "/>
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000_ "/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -706,7 +731,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -719,25 +744,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1070,881 +1098,881 @@
     <col min="1" max="1" width="17.3888888888889" customWidth="1"/>
     <col min="2" max="2" width="30.1111111111111" customWidth="1"/>
     <col min="3" max="3" width="28.5555555555556" customWidth="1"/>
-    <col min="4" max="4" width="19.3055555555556" style="7" customWidth="1"/>
-    <col min="5" max="5" width="20.6111111111111" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3055555555556" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6111111111111" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>10</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>25</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>100</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>0.7455</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="7">
         <v>5.4</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="6">
         <v>0.5983</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="6">
         <v>0.7525</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="6">
         <v>0.7472</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6">
         <v>0.6545</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>25</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>200</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="6">
         <v>0.9121</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="7">
         <v>12.1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6">
         <v>0.7536</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6">
         <v>0.9479</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="6">
         <v>0.8383</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="6">
         <v>0.9358</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>25</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>300</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="6">
         <v>0.9591</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="6">
         <v>0.9515</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="6">
         <v>0.9787</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="6">
         <v>0.9706</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="6">
         <v>0.9819</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>10</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>25</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>500</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="6">
         <v>0.9959</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="7">
         <v>18.5</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="5"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="6">
         <v>0.9946</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="6">
         <v>0.9791</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="6">
         <v>0.9876</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>10</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>25</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>1000</v>
       </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5">
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7">
         <v>28.2</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4">
-        <v>1</v>
-      </c>
-      <c r="E24" s="5"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" s="5"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="5"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>10</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>25</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>1500</v>
       </c>
-      <c r="D27" s="4">
-        <v>1</v>
-      </c>
-      <c r="E27" s="5">
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7">
         <v>39.8</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="6">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4">
-        <v>1</v>
-      </c>
-      <c r="E29" s="5"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="6">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4">
-        <v>1</v>
-      </c>
-      <c r="E30" s="5"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4">
-        <v>1</v>
-      </c>
-      <c r="E31" s="5"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="6">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>10</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>25</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>2000</v>
       </c>
-      <c r="D32" s="4">
-        <v>1</v>
-      </c>
-      <c r="E32" s="5">
+      <c r="D32" s="6">
+        <v>1</v>
+      </c>
+      <c r="E32" s="7">
         <v>52.6</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4">
-        <v>1</v>
-      </c>
-      <c r="E33" s="5"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="6">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="5"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="6">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="4">
-        <v>1</v>
-      </c>
-      <c r="E35" s="5"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="6">
+        <v>1</v>
+      </c>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4">
-        <v>1</v>
-      </c>
-      <c r="E36" s="5"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="6">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>10</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>25</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>2500</v>
       </c>
-      <c r="D37" s="4">
-        <v>1</v>
-      </c>
-      <c r="E37" s="5">
+      <c r="D37" s="6">
+        <v>1</v>
+      </c>
+      <c r="E37" s="7">
         <v>63.3</v>
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="4">
-        <v>1</v>
-      </c>
-      <c r="E39" s="5"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="6">
+        <v>1</v>
+      </c>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="4">
-        <v>1</v>
-      </c>
-      <c r="E40" s="5"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="6">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="4">
-        <v>1</v>
-      </c>
-      <c r="E41" s="5"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="6">
+        <v>1</v>
+      </c>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="3">
+      <c r="A42" s="2">
         <v>10</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>25</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>3000</v>
       </c>
-      <c r="D42" s="4">
-        <v>1</v>
-      </c>
-      <c r="E42" s="5">
+      <c r="D42" s="6">
+        <v>1</v>
+      </c>
+      <c r="E42" s="7">
         <v>74.3</v>
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
-      <c r="E43" s="5"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="6">
+        <v>1</v>
+      </c>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="4">
-        <v>1</v>
-      </c>
-      <c r="E44" s="5"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="6">
+        <v>1</v>
+      </c>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="4">
-        <v>1</v>
-      </c>
-      <c r="E45" s="5"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="6">
+        <v>1</v>
+      </c>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="4">
-        <v>1</v>
-      </c>
-      <c r="E46" s="5"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="6">
+        <v>1</v>
+      </c>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="3">
+      <c r="A47" s="2">
         <v>10</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>25</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>5000</v>
       </c>
-      <c r="D47" s="4">
-        <v>1</v>
-      </c>
-      <c r="E47" s="5">
+      <c r="D47" s="6">
+        <v>1</v>
+      </c>
+      <c r="E47" s="7">
         <v>113.7</v>
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="4">
-        <v>1</v>
-      </c>
-      <c r="E48" s="5"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="6">
+        <v>1</v>
+      </c>
+      <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="4">
-        <v>1</v>
-      </c>
-      <c r="E49" s="5"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="6">
+        <v>1</v>
+      </c>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="4">
-        <v>1</v>
-      </c>
-      <c r="E50" s="5"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="6">
+        <v>1</v>
+      </c>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="4">
-        <v>1</v>
-      </c>
-      <c r="E51" s="5"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="6">
+        <v>1</v>
+      </c>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="3">
+      <c r="A52" s="2">
         <v>10</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>25</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <v>10000</v>
       </c>
-      <c r="D52" s="4">
-        <v>1</v>
-      </c>
-      <c r="E52" s="5">
+      <c r="D52" s="6">
+        <v>1</v>
+      </c>
+      <c r="E52" s="7">
         <v>221.3</v>
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="4">
-        <v>1</v>
-      </c>
-      <c r="E53" s="5"/>
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="6">
+        <v>1</v>
+      </c>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="4">
-        <v>1</v>
-      </c>
-      <c r="E54" s="5"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="6">
+        <v>1</v>
+      </c>
+      <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="4">
-        <v>1</v>
-      </c>
-      <c r="E55" s="5"/>
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="6">
+        <v>1</v>
+      </c>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="4">
-        <v>1</v>
-      </c>
-      <c r="E56" s="5"/>
-    </row>
-    <row r="57" s="6" customFormat="1" spans="1:5">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="10"/>
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="6">
+        <v>1</v>
+      </c>
+      <c r="E56" s="7"/>
+    </row>
+    <row r="57" s="8" customFormat="1" spans="1:5">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="11"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="3">
+      <c r="A58" s="2">
         <v>2</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <v>125</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="2">
         <v>2500</v>
       </c>
-      <c r="D58" s="4">
-        <v>1</v>
-      </c>
-      <c r="E58" s="5">
+      <c r="D58" s="6">
+        <v>1</v>
+      </c>
+      <c r="E58" s="7">
         <v>106.4</v>
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="4">
-        <v>1</v>
-      </c>
-      <c r="E59" s="5"/>
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="6">
+        <v>1</v>
+      </c>
+      <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="4">
-        <v>1</v>
-      </c>
-      <c r="E60" s="5"/>
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="6">
+        <v>1</v>
+      </c>
+      <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="4">
-        <v>1</v>
-      </c>
-      <c r="E61" s="5"/>
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="6">
+        <v>1</v>
+      </c>
+      <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="4">
-        <v>1</v>
-      </c>
-      <c r="E62" s="5"/>
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="6">
+        <v>1</v>
+      </c>
+      <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="3">
+      <c r="A63" s="2">
         <v>5</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="2">
         <v>50</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="2">
         <v>2500</v>
       </c>
-      <c r="D63" s="4">
-        <v>1</v>
-      </c>
-      <c r="E63" s="5">
+      <c r="D63" s="6">
+        <v>1</v>
+      </c>
+      <c r="E63" s="7">
         <v>77.1</v>
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="4">
-        <v>1</v>
-      </c>
-      <c r="E64" s="5"/>
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="6">
+        <v>1</v>
+      </c>
+      <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="4">
-        <v>1</v>
-      </c>
-      <c r="E65" s="5"/>
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="6">
+        <v>1</v>
+      </c>
+      <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="4">
-        <v>1</v>
-      </c>
-      <c r="E66" s="5"/>
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="6">
+        <v>1</v>
+      </c>
+      <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="4">
-        <v>1</v>
-      </c>
-      <c r="E67" s="5"/>
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="6">
+        <v>1</v>
+      </c>
+      <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="3">
+      <c r="A68" s="2">
         <v>10</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="2">
         <v>25</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="2">
         <v>2500</v>
       </c>
-      <c r="D68" s="4">
-        <v>1</v>
-      </c>
-      <c r="E68" s="5">
+      <c r="D68" s="6">
+        <v>1</v>
+      </c>
+      <c r="E68" s="7">
         <v>63.3</v>
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="4">
-        <v>1</v>
-      </c>
-      <c r="E69" s="5"/>
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="6">
+        <v>1</v>
+      </c>
+      <c r="E69" s="7"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="4">
-        <v>1</v>
-      </c>
-      <c r="E70" s="5"/>
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="6">
+        <v>1</v>
+      </c>
+      <c r="E70" s="7"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="4">
-        <v>1</v>
-      </c>
-      <c r="E71" s="5"/>
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="6">
+        <v>1</v>
+      </c>
+      <c r="E71" s="7"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="4">
-        <v>1</v>
-      </c>
-      <c r="E72" s="5"/>
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="6">
+        <v>1</v>
+      </c>
+      <c r="E72" s="7"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="3">
+      <c r="A73" s="2">
         <v>50</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="2">
         <v>5</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="2">
         <v>2500</v>
       </c>
-      <c r="D73" s="4">
-        <v>1</v>
-      </c>
-      <c r="E73" s="5">
+      <c r="D73" s="6">
+        <v>1</v>
+      </c>
+      <c r="E73" s="7">
         <v>189.1</v>
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="4">
-        <v>1</v>
-      </c>
-      <c r="E74" s="5"/>
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="6">
+        <v>1</v>
+      </c>
+      <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="4">
-        <v>1</v>
-      </c>
-      <c r="E75" s="5"/>
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="6">
+        <v>1</v>
+      </c>
+      <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="4">
-        <v>1</v>
-      </c>
-      <c r="E76" s="5"/>
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="6">
+        <v>1</v>
+      </c>
+      <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="4">
-        <v>1</v>
-      </c>
-      <c r="E77" s="5"/>
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="6">
+        <v>1</v>
+      </c>
+      <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="3">
+      <c r="A78" s="2">
         <v>125</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="2">
         <v>2</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="2">
         <v>2500</v>
       </c>
-      <c r="D78" s="4">
-        <v>1</v>
-      </c>
-      <c r="E78" s="5">
+      <c r="D78" s="6">
+        <v>1</v>
+      </c>
+      <c r="E78" s="7">
         <v>221.4</v>
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="4">
-        <v>1</v>
-      </c>
-      <c r="E79" s="5"/>
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="6">
+        <v>1</v>
+      </c>
+      <c r="E79" s="7"/>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="4">
-        <v>1</v>
-      </c>
-      <c r="E80" s="5"/>
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="6">
+        <v>1</v>
+      </c>
+      <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="4">
-        <v>1</v>
-      </c>
-      <c r="E81" s="5"/>
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="6">
+        <v>1</v>
+      </c>
+      <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="4">
-        <v>1</v>
-      </c>
-      <c r="E82" s="5"/>
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="6">
+        <v>1</v>
+      </c>
+      <c r="E82" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="64">
@@ -2024,139 +2052,139 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A1" sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="16.1481481481481" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.2222222222222" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.3055555555556" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.03703703703704" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.2592592592593" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.88888888888889" style="4"/>
-    <col min="7" max="7" width="11.4074074074074" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.88888888888889" style="4"/>
+    <col min="1" max="1" width="16.1481481481481" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.2222222222222" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.3055555555556" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.03703703703704" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.2592592592593" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.88888888888889" style="6"/>
+    <col min="7" max="7" width="11.4074074074074" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.88888888888889" style="6"/>
     <col min="9" max="9" width="12.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" spans="4:9">
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>20</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>25</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>2500</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="6">
         <v>0.8597</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>30.5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="6">
         <v>0.9281</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>220.1</v>
       </c>
-      <c r="H3" s="4">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
         <v>337.8</v>
       </c>
     </row>
     <row r="4" spans="4:9">
-      <c r="D4" s="4">
+      <c r="D4" s="6">
         <v>0.8833</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="6">
         <v>0.9623</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="6">
         <v>0.9965</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="4:9">
-      <c r="D5" s="4">
+      <c r="D5" s="6">
         <v>0.8277</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="6">
         <v>0.9817</v>
       </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3"/>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="4:9">
-      <c r="D6" s="4">
+      <c r="D6" s="6">
         <v>0.842</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="6">
         <v>0.9813</v>
       </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3"/>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="4:9">
-      <c r="D7" s="4">
+      <c r="D7" s="6">
         <v>0.8757</v>
       </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3"/>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2189,52 +2217,52 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="18.3888888888889" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.1574074074074" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.3333333333333" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.3888888888889" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.1574074074074" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.3333333333333" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>0.7859</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>3897.5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>0.8409</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>4079.1</v>
       </c>
     </row>
@@ -2249,7 +2277,7 @@
   <sheetPr/>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2258,7 +2286,7 @@
     <col min="1" max="1" width="20.8333333333333" customWidth="1"/>
     <col min="2" max="2" width="16.3888888888889" customWidth="1"/>
     <col min="3" max="3" width="17.2314814814815" customWidth="1"/>
-    <col min="4" max="4" width="17.3888888888889" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.3888888888889" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2271,12 +2299,12 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
@@ -2285,48 +2313,48 @@
       <c r="C2">
         <v>0.8315</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="5">
         <v>1064.8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3">
         <v>0.8466</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <v>2324</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4">
         <v>0.8189</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>2297.6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="C5">
         <v>0.8181</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>2255.6</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
@@ -2335,43 +2363,43 @@
       <c r="C6">
         <v>0.7953</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>1576.9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
         <v>0.7872</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>2879.3</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8">
         <v>0.8209</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="5">
         <v>2601.1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9">
         <v>0.7857</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <v>2878.4</v>
       </c>
     </row>
@@ -2383,4 +2411,376 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="20.6111111111111" customWidth="1"/>
+    <col min="3" max="3" width="17.1574074074074" customWidth="1"/>
+    <col min="4" max="4" width="26.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="11.3333333333333" style="1"/>
+    <col min="6" max="6" width="17.2407407407407" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2500</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>336.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>110.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2500</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>110.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2500</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>110.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2500</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.9562</v>
+      </c>
+      <c r="F22" s="3">
+        <v>145.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4">
+        <v>0.958</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4">
+        <v>0.9665</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4">
+        <v>0.946</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4">
+        <v>0.9697</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="F12:F16"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="F22:F26"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>